<commit_message>
Update action list template
</commit_message>
<xml_diff>
--- a/assets/Action list template.xlsx
+++ b/assets/Action list template.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20176054\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cverhoosel/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69582189-9A2B-E24F-883D-22B421FA618B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10632" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25440" windowHeight="13240" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Action list" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">'Action list'!$B$2:$H$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Action list'!$B$1:$H$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Action list'!$B$1:$H$26</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>NO.</t>
   </si>
@@ -78,15 +79,6 @@
     <t xml:space="preserve">It is the responsibility of the group to keep the action list up-to-date and available in the group's folder. Note that any pre-listed action items are mandatory for all groups. </t>
   </si>
   <si>
-    <t>Purchase Measurement Training Toolkit</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Before measurement training practical session </t>
-  </si>
-  <si>
     <t>4a</t>
   </si>
   <si>
@@ -111,12 +103,6 @@
     <t>Before tutor meeting wk 4</t>
   </si>
   <si>
-    <t>5a</t>
-  </si>
-  <si>
-    <t>5b</t>
-  </si>
-  <si>
     <t>Prepare final peer review form</t>
   </si>
   <si>
@@ -134,15 +120,21 @@
   <si>
     <t>[Not started / In progress (XX%) / Completed] - Notes</t>
   </si>
+  <si>
+    <t>3a</t>
+  </si>
+  <si>
+    <t>3b</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="d\-m;@"/>
+    <numFmt numFmtId="164" formatCode="d\-m;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -217,13 +209,6 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
-    <font>
-      <i/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -289,60 +274,56 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -350,18 +331,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -704,35 +674,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF44546A"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AML29"/>
+  <dimension ref="A1:AML28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.3984375" style="3"/>
-    <col min="2" max="2" width="9.19921875" style="4"/>
-    <col min="3" max="3" width="34.19921875" style="4"/>
-    <col min="4" max="4" width="23.796875" style="4"/>
-    <col min="5" max="5" width="18.59765625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.8984375" style="4"/>
-    <col min="7" max="7" width="17.09765625" style="4"/>
-    <col min="8" max="8" width="75.09765625" style="4"/>
-    <col min="9" max="9" width="3.3984375" style="3"/>
-    <col min="10" max="13" width="11.296875" style="3"/>
-    <col min="14" max="1026" width="11.296875" style="4"/>
-    <col min="1027" max="16384" width="8.796875" style="1"/>
+    <col min="1" max="1" width="3.33203125" style="3"/>
+    <col min="2" max="2" width="9.1640625" style="4"/>
+    <col min="3" max="3" width="34.1640625" style="4"/>
+    <col min="4" max="4" width="23.83203125" style="4"/>
+    <col min="5" max="5" width="18.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" style="4"/>
+    <col min="7" max="7" width="17.1640625" style="4"/>
+    <col min="8" max="8" width="75.1640625" style="4"/>
+    <col min="9" max="9" width="3.33203125" style="3"/>
+    <col min="10" max="13" width="11.33203125" style="3"/>
+    <col min="14" max="1026" width="11.33203125" style="4"/>
+    <col min="1027" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1025" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1025" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>7</v>
@@ -1763,7 +1733,7 @@
       <c r="AMJ1" s="1"/>
       <c r="AMK1" s="1"/>
     </row>
-    <row r="2" spans="1:1025" s="7" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1025" s="7" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -1792,9 +1762,9 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
     </row>
-    <row r="3" spans="1:1025" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1025" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8"/>
-      <c r="B3" s="15">
+      <c r="B3" s="14">
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -1803,17 +1773,17 @@
       <c r="D3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="16" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="9">
         <v>44074</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="16" t="s">
-        <v>34</v>
+      <c r="H3" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -1821,24 +1791,24 @@
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
     </row>
-    <row r="4" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
-      <c r="B4" s="15">
+      <c r="B4" s="14">
         <v>2</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="16" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="9">
         <v>44074</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="15" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="9"/>
@@ -2860,25 +2830,25 @@
       <c r="AMJ4" s="1"/>
       <c r="AMK4" s="1"/>
     </row>
-    <row r="5" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
-      <c r="B5" s="15">
-        <v>3</v>
+      <c r="B5" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>17</v>
+      <c r="E5" s="16" t="s">
+        <v>12</v>
       </c>
-      <c r="F5" s="9">
-        <v>44074</v>
+      <c r="F5" s="15" t="s">
+        <v>21</v>
       </c>
-      <c r="G5" s="19" t="s">
-        <v>18</v>
+      <c r="G5" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="8"/>
@@ -3899,25 +3869,25 @@
       <c r="AMJ5" s="1"/>
       <c r="AMK5" s="1"/>
     </row>
-    <row r="6" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>9</v>
+      <c r="F6" s="15" t="s">
+        <v>21</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>25</v>
+      <c r="G6" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="8"/>
@@ -4938,25 +4908,25 @@
       <c r="AMJ6" s="1"/>
       <c r="AMK6" s="1"/>
     </row>
-    <row r="7" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
-      <c r="B7" s="15" t="s">
-        <v>21</v>
+      <c r="B7" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="D7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>26</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="8"/>
@@ -5977,25 +5947,25 @@
       <c r="AMJ7" s="1"/>
       <c r="AMK7" s="1"/>
     </row>
-    <row r="8" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
-      <c r="B8" s="15" t="s">
-        <v>27</v>
+      <c r="B8" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>9</v>
+      <c r="D8" s="15" t="s">
+        <v>11</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>12</v>
+      <c r="E8" s="16" t="s">
+        <v>20</v>
       </c>
-      <c r="F8" s="16" t="s">
-        <v>31</v>
+      <c r="F8" s="15" t="s">
+        <v>26</v>
       </c>
-      <c r="G8" s="16" t="s">
-        <v>25</v>
+      <c r="G8" s="15" t="s">
+        <v>27</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="8"/>
@@ -7016,26 +6986,14 @@
       <c r="AMJ8" s="1"/>
       <c r="AMK8" s="1"/>
     </row>
-    <row r="9" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
-      <c r="B9" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>32</v>
-      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -8055,12 +8013,12 @@
       <c r="AMJ9" s="1"/>
       <c r="AMK9" s="1"/>
     </row>
-    <row r="10" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
-      <c r="B10" s="15"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
-      <c r="E10" s="18"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
@@ -9082,12 +9040,12 @@
       <c r="AMJ10" s="1"/>
       <c r="AMK10" s="1"/>
     </row>
-    <row r="11" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
-      <c r="B11" s="15"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="18"/>
+      <c r="E11" s="16"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
@@ -10109,12 +10067,12 @@
       <c r="AMJ11" s="1"/>
       <c r="AMK11" s="1"/>
     </row>
-    <row r="12" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
-      <c r="B12" s="15"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="18"/>
+      <c r="E12" s="16"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -11136,12 +11094,12 @@
       <c r="AMJ12" s="1"/>
       <c r="AMK12" s="1"/>
     </row>
-    <row r="13" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
-      <c r="B13" s="15"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="18"/>
+      <c r="E13" s="16"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -12163,12 +12121,12 @@
       <c r="AMJ13" s="1"/>
       <c r="AMK13" s="1"/>
     </row>
-    <row r="14" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
-      <c r="B14" s="15"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="18"/>
+      <c r="E14" s="16"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -13190,12 +13148,12 @@
       <c r="AMJ14" s="1"/>
       <c r="AMK14" s="1"/>
     </row>
-    <row r="15" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
-      <c r="B15" s="15"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="18"/>
+      <c r="E15" s="16"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -14217,12 +14175,12 @@
       <c r="AMJ15" s="1"/>
       <c r="AMK15" s="1"/>
     </row>
-    <row r="16" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
-      <c r="B16" s="15"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="18"/>
+      <c r="E16" s="16"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
@@ -15244,12 +15202,12 @@
       <c r="AMJ16" s="1"/>
       <c r="AMK16" s="1"/>
     </row>
-    <row r="17" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
-      <c r="B17" s="15"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="18"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
@@ -16271,12 +16229,12 @@
       <c r="AMJ17" s="1"/>
       <c r="AMK17" s="1"/>
     </row>
-    <row r="18" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
-      <c r="B18" s="15"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="18"/>
+      <c r="E18" s="16"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
@@ -17298,12 +17256,12 @@
       <c r="AMJ18" s="1"/>
       <c r="AMK18" s="1"/>
     </row>
-    <row r="19" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
-      <c r="B19" s="15"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
-      <c r="E19" s="18"/>
+      <c r="E19" s="16"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
@@ -18325,12 +18283,12 @@
       <c r="AMJ19" s="1"/>
       <c r="AMK19" s="1"/>
     </row>
-    <row r="20" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
-      <c r="B20" s="15"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="18"/>
+      <c r="E20" s="16"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
@@ -19352,12 +19310,12 @@
       <c r="AMJ20" s="1"/>
       <c r="AMK20" s="1"/>
     </row>
-    <row r="21" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
-      <c r="B21" s="15"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="18"/>
+      <c r="E21" s="16"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
@@ -20379,12 +20337,12 @@
       <c r="AMJ21" s="1"/>
       <c r="AMK21" s="1"/>
     </row>
-    <row r="22" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
-      <c r="B22" s="15"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
-      <c r="E22" s="18"/>
+      <c r="E22" s="16"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
@@ -21406,12 +21364,12 @@
       <c r="AMJ22" s="1"/>
       <c r="AMK22" s="1"/>
     </row>
-    <row r="23" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
-      <c r="B23" s="15"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
-      <c r="E23" s="18"/>
+      <c r="E23" s="16"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -22433,12 +22391,12 @@
       <c r="AMJ23" s="1"/>
       <c r="AMK23" s="1"/>
     </row>
-    <row r="24" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
-      <c r="B24" s="15"/>
+      <c r="B24" s="14"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
-      <c r="E24" s="18"/>
+      <c r="E24" s="16"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
@@ -23460,12 +23418,12 @@
       <c r="AMJ24" s="1"/>
       <c r="AMK24" s="1"/>
     </row>
-    <row r="25" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
-      <c r="B25" s="15"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
-      <c r="E25" s="18"/>
+      <c r="E25" s="16"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -24487,12 +24445,12 @@
       <c r="AMJ25" s="1"/>
       <c r="AMK25" s="1"/>
     </row>
-    <row r="26" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
-      <c r="B26" s="15"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
-      <c r="E26" s="18"/>
+      <c r="E26" s="16"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
@@ -25514,20 +25472,20 @@
       <c r="AMJ26" s="1"/>
       <c r="AMK26" s="1"/>
     </row>
-    <row r="27" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
+    <row r="27" spans="1:1025" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -26541,15 +26499,15 @@
       <c r="AMJ27" s="1"/>
       <c r="AMK27" s="1"/>
     </row>
-    <row r="28" spans="1:1025" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+    <row r="28" spans="1:1025" s="13" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -26559,1036 +26517,9 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
-      <c r="X28" s="1"/>
-      <c r="Y28" s="1"/>
-      <c r="Z28" s="1"/>
-      <c r="AA28" s="1"/>
-      <c r="AB28" s="1"/>
-      <c r="AC28" s="1"/>
-      <c r="AD28" s="1"/>
-      <c r="AE28" s="1"/>
-      <c r="AF28" s="1"/>
-      <c r="AG28" s="1"/>
-      <c r="AH28" s="1"/>
-      <c r="AI28" s="1"/>
-      <c r="AJ28" s="1"/>
-      <c r="AK28" s="1"/>
-      <c r="AL28" s="1"/>
-      <c r="AM28" s="1"/>
-      <c r="AN28" s="1"/>
-      <c r="AO28" s="1"/>
-      <c r="AP28" s="1"/>
-      <c r="AQ28" s="1"/>
-      <c r="AR28" s="1"/>
-      <c r="AS28" s="1"/>
-      <c r="AT28" s="1"/>
-      <c r="AU28" s="1"/>
-      <c r="AV28" s="1"/>
-      <c r="AW28" s="1"/>
-      <c r="AX28" s="1"/>
-      <c r="AY28" s="1"/>
-      <c r="AZ28" s="1"/>
-      <c r="BA28" s="1"/>
-      <c r="BB28" s="1"/>
-      <c r="BC28" s="1"/>
-      <c r="BD28" s="1"/>
-      <c r="BE28" s="1"/>
-      <c r="BF28" s="1"/>
-      <c r="BG28" s="1"/>
-      <c r="BH28" s="1"/>
-      <c r="BI28" s="1"/>
-      <c r="BJ28" s="1"/>
-      <c r="BK28" s="1"/>
-      <c r="BL28" s="1"/>
-      <c r="BM28" s="1"/>
-      <c r="BN28" s="1"/>
-      <c r="BO28" s="1"/>
-      <c r="BP28" s="1"/>
-      <c r="BQ28" s="1"/>
-      <c r="BR28" s="1"/>
-      <c r="BS28" s="1"/>
-      <c r="BT28" s="1"/>
-      <c r="BU28" s="1"/>
-      <c r="BV28" s="1"/>
-      <c r="BW28" s="1"/>
-      <c r="BX28" s="1"/>
-      <c r="BY28" s="1"/>
-      <c r="BZ28" s="1"/>
-      <c r="CA28" s="1"/>
-      <c r="CB28" s="1"/>
-      <c r="CC28" s="1"/>
-      <c r="CD28" s="1"/>
-      <c r="CE28" s="1"/>
-      <c r="CF28" s="1"/>
-      <c r="CG28" s="1"/>
-      <c r="CH28" s="1"/>
-      <c r="CI28" s="1"/>
-      <c r="CJ28" s="1"/>
-      <c r="CK28" s="1"/>
-      <c r="CL28" s="1"/>
-      <c r="CM28" s="1"/>
-      <c r="CN28" s="1"/>
-      <c r="CO28" s="1"/>
-      <c r="CP28" s="1"/>
-      <c r="CQ28" s="1"/>
-      <c r="CR28" s="1"/>
-      <c r="CS28" s="1"/>
-      <c r="CT28" s="1"/>
-      <c r="CU28" s="1"/>
-      <c r="CV28" s="1"/>
-      <c r="CW28" s="1"/>
-      <c r="CX28" s="1"/>
-      <c r="CY28" s="1"/>
-      <c r="CZ28" s="1"/>
-      <c r="DA28" s="1"/>
-      <c r="DB28" s="1"/>
-      <c r="DC28" s="1"/>
-      <c r="DD28" s="1"/>
-      <c r="DE28" s="1"/>
-      <c r="DF28" s="1"/>
-      <c r="DG28" s="1"/>
-      <c r="DH28" s="1"/>
-      <c r="DI28" s="1"/>
-      <c r="DJ28" s="1"/>
-      <c r="DK28" s="1"/>
-      <c r="DL28" s="1"/>
-      <c r="DM28" s="1"/>
-      <c r="DN28" s="1"/>
-      <c r="DO28" s="1"/>
-      <c r="DP28" s="1"/>
-      <c r="DQ28" s="1"/>
-      <c r="DR28" s="1"/>
-      <c r="DS28" s="1"/>
-      <c r="DT28" s="1"/>
-      <c r="DU28" s="1"/>
-      <c r="DV28" s="1"/>
-      <c r="DW28" s="1"/>
-      <c r="DX28" s="1"/>
-      <c r="DY28" s="1"/>
-      <c r="DZ28" s="1"/>
-      <c r="EA28" s="1"/>
-      <c r="EB28" s="1"/>
-      <c r="EC28" s="1"/>
-      <c r="ED28" s="1"/>
-      <c r="EE28" s="1"/>
-      <c r="EF28" s="1"/>
-      <c r="EG28" s="1"/>
-      <c r="EH28" s="1"/>
-      <c r="EI28" s="1"/>
-      <c r="EJ28" s="1"/>
-      <c r="EK28" s="1"/>
-      <c r="EL28" s="1"/>
-      <c r="EM28" s="1"/>
-      <c r="EN28" s="1"/>
-      <c r="EO28" s="1"/>
-      <c r="EP28" s="1"/>
-      <c r="EQ28" s="1"/>
-      <c r="ER28" s="1"/>
-      <c r="ES28" s="1"/>
-      <c r="ET28" s="1"/>
-      <c r="EU28" s="1"/>
-      <c r="EV28" s="1"/>
-      <c r="EW28" s="1"/>
-      <c r="EX28" s="1"/>
-      <c r="EY28" s="1"/>
-      <c r="EZ28" s="1"/>
-      <c r="FA28" s="1"/>
-      <c r="FB28" s="1"/>
-      <c r="FC28" s="1"/>
-      <c r="FD28" s="1"/>
-      <c r="FE28" s="1"/>
-      <c r="FF28" s="1"/>
-      <c r="FG28" s="1"/>
-      <c r="FH28" s="1"/>
-      <c r="FI28" s="1"/>
-      <c r="FJ28" s="1"/>
-      <c r="FK28" s="1"/>
-      <c r="FL28" s="1"/>
-      <c r="FM28" s="1"/>
-      <c r="FN28" s="1"/>
-      <c r="FO28" s="1"/>
-      <c r="FP28" s="1"/>
-      <c r="FQ28" s="1"/>
-      <c r="FR28" s="1"/>
-      <c r="FS28" s="1"/>
-      <c r="FT28" s="1"/>
-      <c r="FU28" s="1"/>
-      <c r="FV28" s="1"/>
-      <c r="FW28" s="1"/>
-      <c r="FX28" s="1"/>
-      <c r="FY28" s="1"/>
-      <c r="FZ28" s="1"/>
-      <c r="GA28" s="1"/>
-      <c r="GB28" s="1"/>
-      <c r="GC28" s="1"/>
-      <c r="GD28" s="1"/>
-      <c r="GE28" s="1"/>
-      <c r="GF28" s="1"/>
-      <c r="GG28" s="1"/>
-      <c r="GH28" s="1"/>
-      <c r="GI28" s="1"/>
-      <c r="GJ28" s="1"/>
-      <c r="GK28" s="1"/>
-      <c r="GL28" s="1"/>
-      <c r="GM28" s="1"/>
-      <c r="GN28" s="1"/>
-      <c r="GO28" s="1"/>
-      <c r="GP28" s="1"/>
-      <c r="GQ28" s="1"/>
-      <c r="GR28" s="1"/>
-      <c r="GS28" s="1"/>
-      <c r="GT28" s="1"/>
-      <c r="GU28" s="1"/>
-      <c r="GV28" s="1"/>
-      <c r="GW28" s="1"/>
-      <c r="GX28" s="1"/>
-      <c r="GY28" s="1"/>
-      <c r="GZ28" s="1"/>
-      <c r="HA28" s="1"/>
-      <c r="HB28" s="1"/>
-      <c r="HC28" s="1"/>
-      <c r="HD28" s="1"/>
-      <c r="HE28" s="1"/>
-      <c r="HF28" s="1"/>
-      <c r="HG28" s="1"/>
-      <c r="HH28" s="1"/>
-      <c r="HI28" s="1"/>
-      <c r="HJ28" s="1"/>
-      <c r="HK28" s="1"/>
-      <c r="HL28" s="1"/>
-      <c r="HM28" s="1"/>
-      <c r="HN28" s="1"/>
-      <c r="HO28" s="1"/>
-      <c r="HP28" s="1"/>
-      <c r="HQ28" s="1"/>
-      <c r="HR28" s="1"/>
-      <c r="HS28" s="1"/>
-      <c r="HT28" s="1"/>
-      <c r="HU28" s="1"/>
-      <c r="HV28" s="1"/>
-      <c r="HW28" s="1"/>
-      <c r="HX28" s="1"/>
-      <c r="HY28" s="1"/>
-      <c r="HZ28" s="1"/>
-      <c r="IA28" s="1"/>
-      <c r="IB28" s="1"/>
-      <c r="IC28" s="1"/>
-      <c r="ID28" s="1"/>
-      <c r="IE28" s="1"/>
-      <c r="IF28" s="1"/>
-      <c r="IG28" s="1"/>
-      <c r="IH28" s="1"/>
-      <c r="II28" s="1"/>
-      <c r="IJ28" s="1"/>
-      <c r="IK28" s="1"/>
-      <c r="IL28" s="1"/>
-      <c r="IM28" s="1"/>
-      <c r="IN28" s="1"/>
-      <c r="IO28" s="1"/>
-      <c r="IP28" s="1"/>
-      <c r="IQ28" s="1"/>
-      <c r="IR28" s="1"/>
-      <c r="IS28" s="1"/>
-      <c r="IT28" s="1"/>
-      <c r="IU28" s="1"/>
-      <c r="IV28" s="1"/>
-      <c r="IW28" s="1"/>
-      <c r="IX28" s="1"/>
-      <c r="IY28" s="1"/>
-      <c r="IZ28" s="1"/>
-      <c r="JA28" s="1"/>
-      <c r="JB28" s="1"/>
-      <c r="JC28" s="1"/>
-      <c r="JD28" s="1"/>
-      <c r="JE28" s="1"/>
-      <c r="JF28" s="1"/>
-      <c r="JG28" s="1"/>
-      <c r="JH28" s="1"/>
-      <c r="JI28" s="1"/>
-      <c r="JJ28" s="1"/>
-      <c r="JK28" s="1"/>
-      <c r="JL28" s="1"/>
-      <c r="JM28" s="1"/>
-      <c r="JN28" s="1"/>
-      <c r="JO28" s="1"/>
-      <c r="JP28" s="1"/>
-      <c r="JQ28" s="1"/>
-      <c r="JR28" s="1"/>
-      <c r="JS28" s="1"/>
-      <c r="JT28" s="1"/>
-      <c r="JU28" s="1"/>
-      <c r="JV28" s="1"/>
-      <c r="JW28" s="1"/>
-      <c r="JX28" s="1"/>
-      <c r="JY28" s="1"/>
-      <c r="JZ28" s="1"/>
-      <c r="KA28" s="1"/>
-      <c r="KB28" s="1"/>
-      <c r="KC28" s="1"/>
-      <c r="KD28" s="1"/>
-      <c r="KE28" s="1"/>
-      <c r="KF28" s="1"/>
-      <c r="KG28" s="1"/>
-      <c r="KH28" s="1"/>
-      <c r="KI28" s="1"/>
-      <c r="KJ28" s="1"/>
-      <c r="KK28" s="1"/>
-      <c r="KL28" s="1"/>
-      <c r="KM28" s="1"/>
-      <c r="KN28" s="1"/>
-      <c r="KO28" s="1"/>
-      <c r="KP28" s="1"/>
-      <c r="KQ28" s="1"/>
-      <c r="KR28" s="1"/>
-      <c r="KS28" s="1"/>
-      <c r="KT28" s="1"/>
-      <c r="KU28" s="1"/>
-      <c r="KV28" s="1"/>
-      <c r="KW28" s="1"/>
-      <c r="KX28" s="1"/>
-      <c r="KY28" s="1"/>
-      <c r="KZ28" s="1"/>
-      <c r="LA28" s="1"/>
-      <c r="LB28" s="1"/>
-      <c r="LC28" s="1"/>
-      <c r="LD28" s="1"/>
-      <c r="LE28" s="1"/>
-      <c r="LF28" s="1"/>
-      <c r="LG28" s="1"/>
-      <c r="LH28" s="1"/>
-      <c r="LI28" s="1"/>
-      <c r="LJ28" s="1"/>
-      <c r="LK28" s="1"/>
-      <c r="LL28" s="1"/>
-      <c r="LM28" s="1"/>
-      <c r="LN28" s="1"/>
-      <c r="LO28" s="1"/>
-      <c r="LP28" s="1"/>
-      <c r="LQ28" s="1"/>
-      <c r="LR28" s="1"/>
-      <c r="LS28" s="1"/>
-      <c r="LT28" s="1"/>
-      <c r="LU28" s="1"/>
-      <c r="LV28" s="1"/>
-      <c r="LW28" s="1"/>
-      <c r="LX28" s="1"/>
-      <c r="LY28" s="1"/>
-      <c r="LZ28" s="1"/>
-      <c r="MA28" s="1"/>
-      <c r="MB28" s="1"/>
-      <c r="MC28" s="1"/>
-      <c r="MD28" s="1"/>
-      <c r="ME28" s="1"/>
-      <c r="MF28" s="1"/>
-      <c r="MG28" s="1"/>
-      <c r="MH28" s="1"/>
-      <c r="MI28" s="1"/>
-      <c r="MJ28" s="1"/>
-      <c r="MK28" s="1"/>
-      <c r="ML28" s="1"/>
-      <c r="MM28" s="1"/>
-      <c r="MN28" s="1"/>
-      <c r="MO28" s="1"/>
-      <c r="MP28" s="1"/>
-      <c r="MQ28" s="1"/>
-      <c r="MR28" s="1"/>
-      <c r="MS28" s="1"/>
-      <c r="MT28" s="1"/>
-      <c r="MU28" s="1"/>
-      <c r="MV28" s="1"/>
-      <c r="MW28" s="1"/>
-      <c r="MX28" s="1"/>
-      <c r="MY28" s="1"/>
-      <c r="MZ28" s="1"/>
-      <c r="NA28" s="1"/>
-      <c r="NB28" s="1"/>
-      <c r="NC28" s="1"/>
-      <c r="ND28" s="1"/>
-      <c r="NE28" s="1"/>
-      <c r="NF28" s="1"/>
-      <c r="NG28" s="1"/>
-      <c r="NH28" s="1"/>
-      <c r="NI28" s="1"/>
-      <c r="NJ28" s="1"/>
-      <c r="NK28" s="1"/>
-      <c r="NL28" s="1"/>
-      <c r="NM28" s="1"/>
-      <c r="NN28" s="1"/>
-      <c r="NO28" s="1"/>
-      <c r="NP28" s="1"/>
-      <c r="NQ28" s="1"/>
-      <c r="NR28" s="1"/>
-      <c r="NS28" s="1"/>
-      <c r="NT28" s="1"/>
-      <c r="NU28" s="1"/>
-      <c r="NV28" s="1"/>
-      <c r="NW28" s="1"/>
-      <c r="NX28" s="1"/>
-      <c r="NY28" s="1"/>
-      <c r="NZ28" s="1"/>
-      <c r="OA28" s="1"/>
-      <c r="OB28" s="1"/>
-      <c r="OC28" s="1"/>
-      <c r="OD28" s="1"/>
-      <c r="OE28" s="1"/>
-      <c r="OF28" s="1"/>
-      <c r="OG28" s="1"/>
-      <c r="OH28" s="1"/>
-      <c r="OI28" s="1"/>
-      <c r="OJ28" s="1"/>
-      <c r="OK28" s="1"/>
-      <c r="OL28" s="1"/>
-      <c r="OM28" s="1"/>
-      <c r="ON28" s="1"/>
-      <c r="OO28" s="1"/>
-      <c r="OP28" s="1"/>
-      <c r="OQ28" s="1"/>
-      <c r="OR28" s="1"/>
-      <c r="OS28" s="1"/>
-      <c r="OT28" s="1"/>
-      <c r="OU28" s="1"/>
-      <c r="OV28" s="1"/>
-      <c r="OW28" s="1"/>
-      <c r="OX28" s="1"/>
-      <c r="OY28" s="1"/>
-      <c r="OZ28" s="1"/>
-      <c r="PA28" s="1"/>
-      <c r="PB28" s="1"/>
-      <c r="PC28" s="1"/>
-      <c r="PD28" s="1"/>
-      <c r="PE28" s="1"/>
-      <c r="PF28" s="1"/>
-      <c r="PG28" s="1"/>
-      <c r="PH28" s="1"/>
-      <c r="PI28" s="1"/>
-      <c r="PJ28" s="1"/>
-      <c r="PK28" s="1"/>
-      <c r="PL28" s="1"/>
-      <c r="PM28" s="1"/>
-      <c r="PN28" s="1"/>
-      <c r="PO28" s="1"/>
-      <c r="PP28" s="1"/>
-      <c r="PQ28" s="1"/>
-      <c r="PR28" s="1"/>
-      <c r="PS28" s="1"/>
-      <c r="PT28" s="1"/>
-      <c r="PU28" s="1"/>
-      <c r="PV28" s="1"/>
-      <c r="PW28" s="1"/>
-      <c r="PX28" s="1"/>
-      <c r="PY28" s="1"/>
-      <c r="PZ28" s="1"/>
-      <c r="QA28" s="1"/>
-      <c r="QB28" s="1"/>
-      <c r="QC28" s="1"/>
-      <c r="QD28" s="1"/>
-      <c r="QE28" s="1"/>
-      <c r="QF28" s="1"/>
-      <c r="QG28" s="1"/>
-      <c r="QH28" s="1"/>
-      <c r="QI28" s="1"/>
-      <c r="QJ28" s="1"/>
-      <c r="QK28" s="1"/>
-      <c r="QL28" s="1"/>
-      <c r="QM28" s="1"/>
-      <c r="QN28" s="1"/>
-      <c r="QO28" s="1"/>
-      <c r="QP28" s="1"/>
-      <c r="QQ28" s="1"/>
-      <c r="QR28" s="1"/>
-      <c r="QS28" s="1"/>
-      <c r="QT28" s="1"/>
-      <c r="QU28" s="1"/>
-      <c r="QV28" s="1"/>
-      <c r="QW28" s="1"/>
-      <c r="QX28" s="1"/>
-      <c r="QY28" s="1"/>
-      <c r="QZ28" s="1"/>
-      <c r="RA28" s="1"/>
-      <c r="RB28" s="1"/>
-      <c r="RC28" s="1"/>
-      <c r="RD28" s="1"/>
-      <c r="RE28" s="1"/>
-      <c r="RF28" s="1"/>
-      <c r="RG28" s="1"/>
-      <c r="RH28" s="1"/>
-      <c r="RI28" s="1"/>
-      <c r="RJ28" s="1"/>
-      <c r="RK28" s="1"/>
-      <c r="RL28" s="1"/>
-      <c r="RM28" s="1"/>
-      <c r="RN28" s="1"/>
-      <c r="RO28" s="1"/>
-      <c r="RP28" s="1"/>
-      <c r="RQ28" s="1"/>
-      <c r="RR28" s="1"/>
-      <c r="RS28" s="1"/>
-      <c r="RT28" s="1"/>
-      <c r="RU28" s="1"/>
-      <c r="RV28" s="1"/>
-      <c r="RW28" s="1"/>
-      <c r="RX28" s="1"/>
-      <c r="RY28" s="1"/>
-      <c r="RZ28" s="1"/>
-      <c r="SA28" s="1"/>
-      <c r="SB28" s="1"/>
-      <c r="SC28" s="1"/>
-      <c r="SD28" s="1"/>
-      <c r="SE28" s="1"/>
-      <c r="SF28" s="1"/>
-      <c r="SG28" s="1"/>
-      <c r="SH28" s="1"/>
-      <c r="SI28" s="1"/>
-      <c r="SJ28" s="1"/>
-      <c r="SK28" s="1"/>
-      <c r="SL28" s="1"/>
-      <c r="SM28" s="1"/>
-      <c r="SN28" s="1"/>
-      <c r="SO28" s="1"/>
-      <c r="SP28" s="1"/>
-      <c r="SQ28" s="1"/>
-      <c r="SR28" s="1"/>
-      <c r="SS28" s="1"/>
-      <c r="ST28" s="1"/>
-      <c r="SU28" s="1"/>
-      <c r="SV28" s="1"/>
-      <c r="SW28" s="1"/>
-      <c r="SX28" s="1"/>
-      <c r="SY28" s="1"/>
-      <c r="SZ28" s="1"/>
-      <c r="TA28" s="1"/>
-      <c r="TB28" s="1"/>
-      <c r="TC28" s="1"/>
-      <c r="TD28" s="1"/>
-      <c r="TE28" s="1"/>
-      <c r="TF28" s="1"/>
-      <c r="TG28" s="1"/>
-      <c r="TH28" s="1"/>
-      <c r="TI28" s="1"/>
-      <c r="TJ28" s="1"/>
-      <c r="TK28" s="1"/>
-      <c r="TL28" s="1"/>
-      <c r="TM28" s="1"/>
-      <c r="TN28" s="1"/>
-      <c r="TO28" s="1"/>
-      <c r="TP28" s="1"/>
-      <c r="TQ28" s="1"/>
-      <c r="TR28" s="1"/>
-      <c r="TS28" s="1"/>
-      <c r="TT28" s="1"/>
-      <c r="TU28" s="1"/>
-      <c r="TV28" s="1"/>
-      <c r="TW28" s="1"/>
-      <c r="TX28" s="1"/>
-      <c r="TY28" s="1"/>
-      <c r="TZ28" s="1"/>
-      <c r="UA28" s="1"/>
-      <c r="UB28" s="1"/>
-      <c r="UC28" s="1"/>
-      <c r="UD28" s="1"/>
-      <c r="UE28" s="1"/>
-      <c r="UF28" s="1"/>
-      <c r="UG28" s="1"/>
-      <c r="UH28" s="1"/>
-      <c r="UI28" s="1"/>
-      <c r="UJ28" s="1"/>
-      <c r="UK28" s="1"/>
-      <c r="UL28" s="1"/>
-      <c r="UM28" s="1"/>
-      <c r="UN28" s="1"/>
-      <c r="UO28" s="1"/>
-      <c r="UP28" s="1"/>
-      <c r="UQ28" s="1"/>
-      <c r="UR28" s="1"/>
-      <c r="US28" s="1"/>
-      <c r="UT28" s="1"/>
-      <c r="UU28" s="1"/>
-      <c r="UV28" s="1"/>
-      <c r="UW28" s="1"/>
-      <c r="UX28" s="1"/>
-      <c r="UY28" s="1"/>
-      <c r="UZ28" s="1"/>
-      <c r="VA28" s="1"/>
-      <c r="VB28" s="1"/>
-      <c r="VC28" s="1"/>
-      <c r="VD28" s="1"/>
-      <c r="VE28" s="1"/>
-      <c r="VF28" s="1"/>
-      <c r="VG28" s="1"/>
-      <c r="VH28" s="1"/>
-      <c r="VI28" s="1"/>
-      <c r="VJ28" s="1"/>
-      <c r="VK28" s="1"/>
-      <c r="VL28" s="1"/>
-      <c r="VM28" s="1"/>
-      <c r="VN28" s="1"/>
-      <c r="VO28" s="1"/>
-      <c r="VP28" s="1"/>
-      <c r="VQ28" s="1"/>
-      <c r="VR28" s="1"/>
-      <c r="VS28" s="1"/>
-      <c r="VT28" s="1"/>
-      <c r="VU28" s="1"/>
-      <c r="VV28" s="1"/>
-      <c r="VW28" s="1"/>
-      <c r="VX28" s="1"/>
-      <c r="VY28" s="1"/>
-      <c r="VZ28" s="1"/>
-      <c r="WA28" s="1"/>
-      <c r="WB28" s="1"/>
-      <c r="WC28" s="1"/>
-      <c r="WD28" s="1"/>
-      <c r="WE28" s="1"/>
-      <c r="WF28" s="1"/>
-      <c r="WG28" s="1"/>
-      <c r="WH28" s="1"/>
-      <c r="WI28" s="1"/>
-      <c r="WJ28" s="1"/>
-      <c r="WK28" s="1"/>
-      <c r="WL28" s="1"/>
-      <c r="WM28" s="1"/>
-      <c r="WN28" s="1"/>
-      <c r="WO28" s="1"/>
-      <c r="WP28" s="1"/>
-      <c r="WQ28" s="1"/>
-      <c r="WR28" s="1"/>
-      <c r="WS28" s="1"/>
-      <c r="WT28" s="1"/>
-      <c r="WU28" s="1"/>
-      <c r="WV28" s="1"/>
-      <c r="WW28" s="1"/>
-      <c r="WX28" s="1"/>
-      <c r="WY28" s="1"/>
-      <c r="WZ28" s="1"/>
-      <c r="XA28" s="1"/>
-      <c r="XB28" s="1"/>
-      <c r="XC28" s="1"/>
-      <c r="XD28" s="1"/>
-      <c r="XE28" s="1"/>
-      <c r="XF28" s="1"/>
-      <c r="XG28" s="1"/>
-      <c r="XH28" s="1"/>
-      <c r="XI28" s="1"/>
-      <c r="XJ28" s="1"/>
-      <c r="XK28" s="1"/>
-      <c r="XL28" s="1"/>
-      <c r="XM28" s="1"/>
-      <c r="XN28" s="1"/>
-      <c r="XO28" s="1"/>
-      <c r="XP28" s="1"/>
-      <c r="XQ28" s="1"/>
-      <c r="XR28" s="1"/>
-      <c r="XS28" s="1"/>
-      <c r="XT28" s="1"/>
-      <c r="XU28" s="1"/>
-      <c r="XV28" s="1"/>
-      <c r="XW28" s="1"/>
-      <c r="XX28" s="1"/>
-      <c r="XY28" s="1"/>
-      <c r="XZ28" s="1"/>
-      <c r="YA28" s="1"/>
-      <c r="YB28" s="1"/>
-      <c r="YC28" s="1"/>
-      <c r="YD28" s="1"/>
-      <c r="YE28" s="1"/>
-      <c r="YF28" s="1"/>
-      <c r="YG28" s="1"/>
-      <c r="YH28" s="1"/>
-      <c r="YI28" s="1"/>
-      <c r="YJ28" s="1"/>
-      <c r="YK28" s="1"/>
-      <c r="YL28" s="1"/>
-      <c r="YM28" s="1"/>
-      <c r="YN28" s="1"/>
-      <c r="YO28" s="1"/>
-      <c r="YP28" s="1"/>
-      <c r="YQ28" s="1"/>
-      <c r="YR28" s="1"/>
-      <c r="YS28" s="1"/>
-      <c r="YT28" s="1"/>
-      <c r="YU28" s="1"/>
-      <c r="YV28" s="1"/>
-      <c r="YW28" s="1"/>
-      <c r="YX28" s="1"/>
-      <c r="YY28" s="1"/>
-      <c r="YZ28" s="1"/>
-      <c r="ZA28" s="1"/>
-      <c r="ZB28" s="1"/>
-      <c r="ZC28" s="1"/>
-      <c r="ZD28" s="1"/>
-      <c r="ZE28" s="1"/>
-      <c r="ZF28" s="1"/>
-      <c r="ZG28" s="1"/>
-      <c r="ZH28" s="1"/>
-      <c r="ZI28" s="1"/>
-      <c r="ZJ28" s="1"/>
-      <c r="ZK28" s="1"/>
-      <c r="ZL28" s="1"/>
-      <c r="ZM28" s="1"/>
-      <c r="ZN28" s="1"/>
-      <c r="ZO28" s="1"/>
-      <c r="ZP28" s="1"/>
-      <c r="ZQ28" s="1"/>
-      <c r="ZR28" s="1"/>
-      <c r="ZS28" s="1"/>
-      <c r="ZT28" s="1"/>
-      <c r="ZU28" s="1"/>
-      <c r="ZV28" s="1"/>
-      <c r="ZW28" s="1"/>
-      <c r="ZX28" s="1"/>
-      <c r="ZY28" s="1"/>
-      <c r="ZZ28" s="1"/>
-      <c r="AAA28" s="1"/>
-      <c r="AAB28" s="1"/>
-      <c r="AAC28" s="1"/>
-      <c r="AAD28" s="1"/>
-      <c r="AAE28" s="1"/>
-      <c r="AAF28" s="1"/>
-      <c r="AAG28" s="1"/>
-      <c r="AAH28" s="1"/>
-      <c r="AAI28" s="1"/>
-      <c r="AAJ28" s="1"/>
-      <c r="AAK28" s="1"/>
-      <c r="AAL28" s="1"/>
-      <c r="AAM28" s="1"/>
-      <c r="AAN28" s="1"/>
-      <c r="AAO28" s="1"/>
-      <c r="AAP28" s="1"/>
-      <c r="AAQ28" s="1"/>
-      <c r="AAR28" s="1"/>
-      <c r="AAS28" s="1"/>
-      <c r="AAT28" s="1"/>
-      <c r="AAU28" s="1"/>
-      <c r="AAV28" s="1"/>
-      <c r="AAW28" s="1"/>
-      <c r="AAX28" s="1"/>
-      <c r="AAY28" s="1"/>
-      <c r="AAZ28" s="1"/>
-      <c r="ABA28" s="1"/>
-      <c r="ABB28" s="1"/>
-      <c r="ABC28" s="1"/>
-      <c r="ABD28" s="1"/>
-      <c r="ABE28" s="1"/>
-      <c r="ABF28" s="1"/>
-      <c r="ABG28" s="1"/>
-      <c r="ABH28" s="1"/>
-      <c r="ABI28" s="1"/>
-      <c r="ABJ28" s="1"/>
-      <c r="ABK28" s="1"/>
-      <c r="ABL28" s="1"/>
-      <c r="ABM28" s="1"/>
-      <c r="ABN28" s="1"/>
-      <c r="ABO28" s="1"/>
-      <c r="ABP28" s="1"/>
-      <c r="ABQ28" s="1"/>
-      <c r="ABR28" s="1"/>
-      <c r="ABS28" s="1"/>
-      <c r="ABT28" s="1"/>
-      <c r="ABU28" s="1"/>
-      <c r="ABV28" s="1"/>
-      <c r="ABW28" s="1"/>
-      <c r="ABX28" s="1"/>
-      <c r="ABY28" s="1"/>
-      <c r="ABZ28" s="1"/>
-      <c r="ACA28" s="1"/>
-      <c r="ACB28" s="1"/>
-      <c r="ACC28" s="1"/>
-      <c r="ACD28" s="1"/>
-      <c r="ACE28" s="1"/>
-      <c r="ACF28" s="1"/>
-      <c r="ACG28" s="1"/>
-      <c r="ACH28" s="1"/>
-      <c r="ACI28" s="1"/>
-      <c r="ACJ28" s="1"/>
-      <c r="ACK28" s="1"/>
-      <c r="ACL28" s="1"/>
-      <c r="ACM28" s="1"/>
-      <c r="ACN28" s="1"/>
-      <c r="ACO28" s="1"/>
-      <c r="ACP28" s="1"/>
-      <c r="ACQ28" s="1"/>
-      <c r="ACR28" s="1"/>
-      <c r="ACS28" s="1"/>
-      <c r="ACT28" s="1"/>
-      <c r="ACU28" s="1"/>
-      <c r="ACV28" s="1"/>
-      <c r="ACW28" s="1"/>
-      <c r="ACX28" s="1"/>
-      <c r="ACY28" s="1"/>
-      <c r="ACZ28" s="1"/>
-      <c r="ADA28" s="1"/>
-      <c r="ADB28" s="1"/>
-      <c r="ADC28" s="1"/>
-      <c r="ADD28" s="1"/>
-      <c r="ADE28" s="1"/>
-      <c r="ADF28" s="1"/>
-      <c r="ADG28" s="1"/>
-      <c r="ADH28" s="1"/>
-      <c r="ADI28" s="1"/>
-      <c r="ADJ28" s="1"/>
-      <c r="ADK28" s="1"/>
-      <c r="ADL28" s="1"/>
-      <c r="ADM28" s="1"/>
-      <c r="ADN28" s="1"/>
-      <c r="ADO28" s="1"/>
-      <c r="ADP28" s="1"/>
-      <c r="ADQ28" s="1"/>
-      <c r="ADR28" s="1"/>
-      <c r="ADS28" s="1"/>
-      <c r="ADT28" s="1"/>
-      <c r="ADU28" s="1"/>
-      <c r="ADV28" s="1"/>
-      <c r="ADW28" s="1"/>
-      <c r="ADX28" s="1"/>
-      <c r="ADY28" s="1"/>
-      <c r="ADZ28" s="1"/>
-      <c r="AEA28" s="1"/>
-      <c r="AEB28" s="1"/>
-      <c r="AEC28" s="1"/>
-      <c r="AED28" s="1"/>
-      <c r="AEE28" s="1"/>
-      <c r="AEF28" s="1"/>
-      <c r="AEG28" s="1"/>
-      <c r="AEH28" s="1"/>
-      <c r="AEI28" s="1"/>
-      <c r="AEJ28" s="1"/>
-      <c r="AEK28" s="1"/>
-      <c r="AEL28" s="1"/>
-      <c r="AEM28" s="1"/>
-      <c r="AEN28" s="1"/>
-      <c r="AEO28" s="1"/>
-      <c r="AEP28" s="1"/>
-      <c r="AEQ28" s="1"/>
-      <c r="AER28" s="1"/>
-      <c r="AES28" s="1"/>
-      <c r="AET28" s="1"/>
-      <c r="AEU28" s="1"/>
-      <c r="AEV28" s="1"/>
-      <c r="AEW28" s="1"/>
-      <c r="AEX28" s="1"/>
-      <c r="AEY28" s="1"/>
-      <c r="AEZ28" s="1"/>
-      <c r="AFA28" s="1"/>
-      <c r="AFB28" s="1"/>
-      <c r="AFC28" s="1"/>
-      <c r="AFD28" s="1"/>
-      <c r="AFE28" s="1"/>
-      <c r="AFF28" s="1"/>
-      <c r="AFG28" s="1"/>
-      <c r="AFH28" s="1"/>
-      <c r="AFI28" s="1"/>
-      <c r="AFJ28" s="1"/>
-      <c r="AFK28" s="1"/>
-      <c r="AFL28" s="1"/>
-      <c r="AFM28" s="1"/>
-      <c r="AFN28" s="1"/>
-      <c r="AFO28" s="1"/>
-      <c r="AFP28" s="1"/>
-      <c r="AFQ28" s="1"/>
-      <c r="AFR28" s="1"/>
-      <c r="AFS28" s="1"/>
-      <c r="AFT28" s="1"/>
-      <c r="AFU28" s="1"/>
-      <c r="AFV28" s="1"/>
-      <c r="AFW28" s="1"/>
-      <c r="AFX28" s="1"/>
-      <c r="AFY28" s="1"/>
-      <c r="AFZ28" s="1"/>
-      <c r="AGA28" s="1"/>
-      <c r="AGB28" s="1"/>
-      <c r="AGC28" s="1"/>
-      <c r="AGD28" s="1"/>
-      <c r="AGE28" s="1"/>
-      <c r="AGF28" s="1"/>
-      <c r="AGG28" s="1"/>
-      <c r="AGH28" s="1"/>
-      <c r="AGI28" s="1"/>
-      <c r="AGJ28" s="1"/>
-      <c r="AGK28" s="1"/>
-      <c r="AGL28" s="1"/>
-      <c r="AGM28" s="1"/>
-      <c r="AGN28" s="1"/>
-      <c r="AGO28" s="1"/>
-      <c r="AGP28" s="1"/>
-      <c r="AGQ28" s="1"/>
-      <c r="AGR28" s="1"/>
-      <c r="AGS28" s="1"/>
-      <c r="AGT28" s="1"/>
-      <c r="AGU28" s="1"/>
-      <c r="AGV28" s="1"/>
-      <c r="AGW28" s="1"/>
-      <c r="AGX28" s="1"/>
-      <c r="AGY28" s="1"/>
-      <c r="AGZ28" s="1"/>
-      <c r="AHA28" s="1"/>
-      <c r="AHB28" s="1"/>
-      <c r="AHC28" s="1"/>
-      <c r="AHD28" s="1"/>
-      <c r="AHE28" s="1"/>
-      <c r="AHF28" s="1"/>
-      <c r="AHG28" s="1"/>
-      <c r="AHH28" s="1"/>
-      <c r="AHI28" s="1"/>
-      <c r="AHJ28" s="1"/>
-      <c r="AHK28" s="1"/>
-      <c r="AHL28" s="1"/>
-      <c r="AHM28" s="1"/>
-      <c r="AHN28" s="1"/>
-      <c r="AHO28" s="1"/>
-      <c r="AHP28" s="1"/>
-      <c r="AHQ28" s="1"/>
-      <c r="AHR28" s="1"/>
-      <c r="AHS28" s="1"/>
-      <c r="AHT28" s="1"/>
-      <c r="AHU28" s="1"/>
-      <c r="AHV28" s="1"/>
-      <c r="AHW28" s="1"/>
-      <c r="AHX28" s="1"/>
-      <c r="AHY28" s="1"/>
-      <c r="AHZ28" s="1"/>
-      <c r="AIA28" s="1"/>
-      <c r="AIB28" s="1"/>
-      <c r="AIC28" s="1"/>
-      <c r="AID28" s="1"/>
-      <c r="AIE28" s="1"/>
-      <c r="AIF28" s="1"/>
-      <c r="AIG28" s="1"/>
-      <c r="AIH28" s="1"/>
-      <c r="AII28" s="1"/>
-      <c r="AIJ28" s="1"/>
-      <c r="AIK28" s="1"/>
-      <c r="AIL28" s="1"/>
-      <c r="AIM28" s="1"/>
-      <c r="AIN28" s="1"/>
-      <c r="AIO28" s="1"/>
-      <c r="AIP28" s="1"/>
-      <c r="AIQ28" s="1"/>
-      <c r="AIR28" s="1"/>
-      <c r="AIS28" s="1"/>
-      <c r="AIT28" s="1"/>
-      <c r="AIU28" s="1"/>
-      <c r="AIV28" s="1"/>
-      <c r="AIW28" s="1"/>
-      <c r="AIX28" s="1"/>
-      <c r="AIY28" s="1"/>
-      <c r="AIZ28" s="1"/>
-      <c r="AJA28" s="1"/>
-      <c r="AJB28" s="1"/>
-      <c r="AJC28" s="1"/>
-      <c r="AJD28" s="1"/>
-      <c r="AJE28" s="1"/>
-      <c r="AJF28" s="1"/>
-      <c r="AJG28" s="1"/>
-      <c r="AJH28" s="1"/>
-      <c r="AJI28" s="1"/>
-      <c r="AJJ28" s="1"/>
-      <c r="AJK28" s="1"/>
-      <c r="AJL28" s="1"/>
-      <c r="AJM28" s="1"/>
-      <c r="AJN28" s="1"/>
-      <c r="AJO28" s="1"/>
-      <c r="AJP28" s="1"/>
-      <c r="AJQ28" s="1"/>
-      <c r="AJR28" s="1"/>
-      <c r="AJS28" s="1"/>
-      <c r="AJT28" s="1"/>
-      <c r="AJU28" s="1"/>
-      <c r="AJV28" s="1"/>
-      <c r="AJW28" s="1"/>
-      <c r="AJX28" s="1"/>
-      <c r="AJY28" s="1"/>
-      <c r="AJZ28" s="1"/>
-      <c r="AKA28" s="1"/>
-      <c r="AKB28" s="1"/>
-      <c r="AKC28" s="1"/>
-      <c r="AKD28" s="1"/>
-      <c r="AKE28" s="1"/>
-      <c r="AKF28" s="1"/>
-      <c r="AKG28" s="1"/>
-      <c r="AKH28" s="1"/>
-      <c r="AKI28" s="1"/>
-      <c r="AKJ28" s="1"/>
-      <c r="AKK28" s="1"/>
-      <c r="AKL28" s="1"/>
-      <c r="AKM28" s="1"/>
-      <c r="AKN28" s="1"/>
-      <c r="AKO28" s="1"/>
-      <c r="AKP28" s="1"/>
-      <c r="AKQ28" s="1"/>
-      <c r="AKR28" s="1"/>
-      <c r="AKS28" s="1"/>
-      <c r="AKT28" s="1"/>
-      <c r="AKU28" s="1"/>
-      <c r="AKV28" s="1"/>
-      <c r="AKW28" s="1"/>
-      <c r="AKX28" s="1"/>
-      <c r="AKY28" s="1"/>
-      <c r="AKZ28" s="1"/>
-      <c r="ALA28" s="1"/>
-      <c r="ALB28" s="1"/>
-      <c r="ALC28" s="1"/>
-      <c r="ALD28" s="1"/>
-      <c r="ALE28" s="1"/>
-      <c r="ALF28" s="1"/>
-      <c r="ALG28" s="1"/>
-      <c r="ALH28" s="1"/>
-      <c r="ALI28" s="1"/>
-      <c r="ALJ28" s="1"/>
-      <c r="ALK28" s="1"/>
-      <c r="ALL28" s="1"/>
-      <c r="ALM28" s="1"/>
-      <c r="ALN28" s="1"/>
-      <c r="ALO28" s="1"/>
-      <c r="ALP28" s="1"/>
-      <c r="ALQ28" s="1"/>
-      <c r="ALR28" s="1"/>
-      <c r="ALS28" s="1"/>
-      <c r="ALT28" s="1"/>
-      <c r="ALU28" s="1"/>
-      <c r="ALV28" s="1"/>
-      <c r="ALW28" s="1"/>
-      <c r="ALX28" s="1"/>
-      <c r="ALY28" s="1"/>
-      <c r="ALZ28" s="1"/>
-      <c r="AMA28" s="1"/>
-      <c r="AMB28" s="1"/>
-      <c r="AMC28" s="1"/>
-      <c r="AMD28" s="1"/>
-      <c r="AME28" s="1"/>
-      <c r="AMF28" s="1"/>
-      <c r="AMG28" s="1"/>
-      <c r="AMH28" s="1"/>
-      <c r="AMI28" s="1"/>
-      <c r="AMJ28" s="1"/>
-      <c r="AMK28" s="1"/>
-    </row>
-    <row r="29" spans="1:1025" s="14" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
-      <c r="P29" s="13"/>
-      <c r="Q29" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:H2"/>
+  <autoFilter ref="B2:H2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="E1:G1"/>
   </mergeCells>

</xml_diff>